<commit_message>
Add sample Excel data with multiple sheets and generation script
Co-authored-by: ramarajan15 <11455808+ramarajan15@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/public/SheetCuttingBusinessTemplate.xlsx
+++ b/public/SheetCuttingBusinessTemplate.xlsx
@@ -3,7 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Sheet Cutting Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Orders" sheetId="1" r:id="rId1"/>
+    <sheet name="Customers" sheetId="2" r:id="rId2"/>
+    <sheet name="Factories" sheetId="3" r:id="rId3"/>
+    <sheet name="Purchases" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -397,279 +400,747 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Material</v>
+        <v>Order Ref</v>
       </c>
       <c r="B1" t="str">
         <v>Date</v>
       </c>
       <c r="C1" t="str">
+        <v>Customer ID</v>
+      </c>
+      <c r="D1" t="str">
         <v>Customer</v>
       </c>
-      <c r="D1" t="str">
-        <v>Order Ref</v>
-      </c>
       <c r="E1" t="str">
+        <v>Sheet ID</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Purchase ID</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Factory ID</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Factory Name</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Batch Ref</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Material</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Piece Size (mm)</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Qty</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Area per Piece (m²)</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Total Area Used (m²)</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Unit Cost</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Unit Sale Price</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>Total Cost</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Total Sale</v>
+      </c>
+      <c r="S1" t="str">
+        <v>Profit</v>
+      </c>
+      <c r="T1" t="str">
+        <v>Leftover Area (m²)</v>
+      </c>
+      <c r="U1" t="str">
+        <v>Offcut Used? (Y/N)</v>
+      </c>
+      <c r="V1" t="str">
         <v>Sheet Used (Y/N)</v>
       </c>
-      <c r="F1" t="str">
-        <v>Piece Size (mm)</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Qty</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Area per Piece (m²)</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Total Area Used (m²)</v>
-      </c>
-      <c r="J1" t="str">
-        <v>Unit Cost</v>
-      </c>
-      <c r="K1" t="str">
-        <v>Unit Sale Price</v>
-      </c>
-      <c r="L1" t="str">
-        <v>Total Cost</v>
-      </c>
-      <c r="M1" t="str">
-        <v>Total Sale</v>
-      </c>
-      <c r="N1" t="str">
-        <v>Profit</v>
-      </c>
-      <c r="O1" t="str">
-        <v>Leftover Area (m²)</v>
-      </c>
-      <c r="P1" t="str">
-        <v>Offcut Used? (Y/N)</v>
-      </c>
-      <c r="Q1" t="str">
+      <c r="W1" t="str">
         <v>Notes</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Plastic</v>
+        <v>ORD001</v>
       </c>
       <c r="B2" t="str">
-        <v>2025-10-01</v>
+        <v>2024-01-16</v>
       </c>
       <c r="C2" t="str">
-        <v>John Doe</v>
+        <v>CUST001</v>
       </c>
       <c r="D2" t="str">
-        <v>ORD001</v>
+        <v>ABC Manufacturing</v>
       </c>
       <c r="E2" t="str">
+        <v>SHT001</v>
+      </c>
+      <c r="F2" t="str">
+        <v>PUR001</v>
+      </c>
+      <c r="G2" t="str">
+        <v>FAC001</v>
+      </c>
+      <c r="H2" t="str">
+        <v>Steel Works Ltd</v>
+      </c>
+      <c r="I2" t="str">
+        <v>BATCH-2024-001</v>
+      </c>
+      <c r="J2" t="str">
+        <v>Stainless Steel</v>
+      </c>
+      <c r="K2" t="str">
+        <v>600x400</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>0.24</v>
+      </c>
+      <c r="N2">
+        <v>2.4</v>
+      </c>
+      <c r="O2">
+        <v>85.5</v>
+      </c>
+      <c r="P2">
+        <v>125</v>
+      </c>
+      <c r="Q2">
+        <v>855</v>
+      </c>
+      <c r="R2">
+        <v>1250</v>
+      </c>
+      <c r="S2">
+        <v>395</v>
+      </c>
+      <c r="T2">
+        <v>0.58</v>
+      </c>
+      <c r="U2" t="str">
+        <v>N</v>
+      </c>
+      <c r="V2" t="str">
         <v>Y</v>
       </c>
-      <c r="F2" t="str">
-        <v>1200x2400</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>2.88</v>
-      </c>
-      <c r="I2">
-        <v>28.8</v>
-      </c>
-      <c r="J2">
-        <v>100</v>
-      </c>
-      <c r="K2">
-        <v>150</v>
-      </c>
-      <c r="L2">
-        <v>1000</v>
-      </c>
-      <c r="M2">
-        <v>1500</v>
-      </c>
-      <c r="N2">
-        <v>500</v>
-      </c>
-      <c r="O2">
-        <v>3.2</v>
-      </c>
-      <c r="P2" t="str">
-        <v>N</v>
-      </c>
-      <c r="Q2" t="str">
-        <v>First order</v>
+      <c r="W2" t="str">
+        <v>Custom cut for ABC Manufacturing</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Hylam</v>
+        <v>ORD002</v>
       </c>
       <c r="B3" t="str">
-        <v>2025-10-02</v>
+        <v>2024-01-22</v>
       </c>
       <c r="C3" t="str">
-        <v>Jane Smith</v>
+        <v>CUST002</v>
       </c>
       <c r="D3" t="str">
-        <v>ORD002</v>
+        <v>XYZ Construction</v>
       </c>
       <c r="E3" t="str">
-        <v>N</v>
+        <v>SHT002</v>
       </c>
       <c r="F3" t="str">
-        <v>1000x2000</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>80</v>
-      </c>
-      <c r="K3">
-        <v>120</v>
+        <v>PUR002</v>
+      </c>
+      <c r="G3" t="str">
+        <v>FAC002</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Aluminum Solutions</v>
+      </c>
+      <c r="I3" t="str">
+        <v>BATCH-2024-002</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Aluminum 6061</v>
+      </c>
+      <c r="K3" t="str">
+        <v>800x600</v>
       </c>
       <c r="L3">
-        <v>400</v>
+        <v>15</v>
       </c>
       <c r="M3">
-        <v>600</v>
+        <v>0.48</v>
       </c>
       <c r="N3">
-        <v>200</v>
+        <v>7.2</v>
       </c>
       <c r="O3">
-        <v>6</v>
-      </c>
-      <c r="P3" t="str">
+        <v>95</v>
+      </c>
+      <c r="P3">
+        <v>140</v>
+      </c>
+      <c r="Q3">
+        <v>1425</v>
+      </c>
+      <c r="R3">
+        <v>2100</v>
+      </c>
+      <c r="S3">
+        <v>675</v>
+      </c>
+      <c r="T3">
+        <v>1.25</v>
+      </c>
+      <c r="U3" t="str">
         <v>Y</v>
       </c>
-      <c r="Q3" t="str">
-        <v>Used offcut</v>
+      <c r="V3" t="str">
+        <v>Y</v>
+      </c>
+      <c r="W3" t="str">
+        <v>Reused leftover for smaller pieces</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Aluminium</v>
+        <v>ORD003</v>
       </c>
       <c r="B4" t="str">
-        <v>2025-10-03</v>
+        <v>2024-02-05</v>
       </c>
       <c r="C4" t="str">
-        <v>Acme Corp</v>
+        <v>CUST003</v>
       </c>
       <c r="D4" t="str">
-        <v>ORD003</v>
+        <v>Tech Solutions Inc</v>
       </c>
       <c r="E4" t="str">
+        <v>SHT003</v>
+      </c>
+      <c r="F4" t="str">
+        <v>PUR003</v>
+      </c>
+      <c r="G4" t="str">
+        <v>FAC001</v>
+      </c>
+      <c r="H4" t="str">
+        <v>Steel Works Ltd</v>
+      </c>
+      <c r="I4" t="str">
+        <v>BATCH-2024-003</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Mild Steel</v>
+      </c>
+      <c r="K4" t="str">
+        <v>1000x800</v>
+      </c>
+      <c r="L4">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <v>0.8</v>
+      </c>
+      <c r="N4">
+        <v>6.4</v>
+      </c>
+      <c r="O4">
+        <v>120</v>
+      </c>
+      <c r="P4">
+        <v>165</v>
+      </c>
+      <c r="Q4">
+        <v>960</v>
+      </c>
+      <c r="R4">
+        <v>1320</v>
+      </c>
+      <c r="S4">
+        <v>360</v>
+      </c>
+      <c r="T4">
+        <v>2.1</v>
+      </c>
+      <c r="U4" t="str">
+        <v>N</v>
+      </c>
+      <c r="V4" t="str">
         <v>Y</v>
       </c>
-      <c r="F4" t="str">
-        <v>1500x3000</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-      <c r="H4">
-        <v>4.5</v>
-      </c>
-      <c r="I4">
-        <v>27</v>
-      </c>
-      <c r="J4">
-        <v>200</v>
-      </c>
-      <c r="K4">
-        <v>270</v>
-      </c>
-      <c r="L4">
-        <v>1200</v>
-      </c>
-      <c r="M4">
-        <v>1620</v>
-      </c>
-      <c r="N4">
-        <v>420</v>
-      </c>
-      <c r="O4">
-        <v>2</v>
-      </c>
-      <c r="P4" t="str">
-        <v>N</v>
-      </c>
-      <c r="Q4" t="str">
-        <v>Big order</v>
+      <c r="W4" t="str">
+        <v>High precision cutting required</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Plywood</v>
+        <v>ORD004</v>
       </c>
       <c r="B5" t="str">
-        <v>2025-10-04</v>
+        <v>2024-02-10</v>
       </c>
       <c r="C5" t="str">
-        <v>Beta Ltd</v>
+        <v>CUST001</v>
       </c>
       <c r="D5" t="str">
-        <v>ORD004</v>
+        <v>ABC Manufacturing</v>
       </c>
       <c r="E5" t="str">
+        <v>SHT001</v>
+      </c>
+      <c r="F5" t="str">
+        <v>PUR001</v>
+      </c>
+      <c r="G5" t="str">
+        <v>FAC001</v>
+      </c>
+      <c r="H5" t="str">
+        <v>Steel Works Ltd</v>
+      </c>
+      <c r="I5" t="str">
+        <v>BATCH-2024-001</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Stainless Steel</v>
+      </c>
+      <c r="K5" t="str">
+        <v>500x300</v>
+      </c>
+      <c r="L5">
+        <v>20</v>
+      </c>
+      <c r="M5">
+        <v>0.15</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>85.5</v>
+      </c>
+      <c r="P5">
+        <v>120</v>
+      </c>
+      <c r="Q5">
+        <v>1710</v>
+      </c>
+      <c r="R5">
+        <v>2400</v>
+      </c>
+      <c r="S5">
+        <v>690</v>
+      </c>
+      <c r="T5">
+        <v>0.98</v>
+      </c>
+      <c r="U5" t="str">
+        <v>N</v>
+      </c>
+      <c r="V5" t="str">
         <v>Y</v>
       </c>
-      <c r="F5" t="str">
-        <v>1220x2440</v>
-      </c>
-      <c r="G5">
-        <v>8</v>
-      </c>
-      <c r="H5">
-        <v>2.9768</v>
-      </c>
-      <c r="I5">
-        <v>23.8144</v>
-      </c>
-      <c r="J5">
-        <v>60</v>
-      </c>
-      <c r="K5">
-        <v>100</v>
-      </c>
-      <c r="L5">
-        <v>480</v>
-      </c>
-      <c r="M5">
-        <v>800</v>
-      </c>
-      <c r="N5">
-        <v>320</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5" t="str">
-        <v>N</v>
-      </c>
-      <c r="Q5" t="str">
-        <v>Standard cut</v>
+      <c r="W5" t="str">
+        <v>Standard order</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:W5"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>email</v>
+      </c>
+      <c r="D1" t="str">
+        <v>phone</v>
+      </c>
+      <c r="E1" t="str">
+        <v>address</v>
+      </c>
+      <c r="F1" t="str">
+        <v>notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>CUST001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>ABC Manufacturing</v>
+      </c>
+      <c r="C2" t="str">
+        <v>contact@abcmfg.com</v>
+      </c>
+      <c r="D2" t="str">
+        <v>+1-555-0101</v>
+      </c>
+      <c r="E2" t="str">
+        <v>123 Industrial Ave, New York, NY</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Regular customer, monthly orders</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>CUST002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>XYZ Construction</v>
+      </c>
+      <c r="C3" t="str">
+        <v>info@xyzconstruction.com</v>
+      </c>
+      <c r="D3" t="str">
+        <v>+1-555-0102</v>
+      </c>
+      <c r="E3" t="str">
+        <v>456 Builder St, Los Angeles, CA</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Large volume orders</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>CUST003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Tech Solutions Inc</v>
+      </c>
+      <c r="C4" t="str">
+        <v>procurement@techsolutions.com</v>
+      </c>
+      <c r="D4" t="str">
+        <v>+1-555-0103</v>
+      </c>
+      <c r="E4" t="str">
+        <v>789 Tech Park, San Francisco, CA</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Specialty materials required</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>location</v>
+      </c>
+      <c r="D1" t="str">
+        <v>contact</v>
+      </c>
+      <c r="E1" t="str">
+        <v>email</v>
+      </c>
+      <c r="F1" t="str">
+        <v>phone</v>
+      </c>
+      <c r="G1" t="str">
+        <v>materials</v>
+      </c>
+      <c r="H1" t="str">
+        <v>notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>FAC001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Steel Works Ltd</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Pittsburgh, PA</v>
+      </c>
+      <c r="D2" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="E2" t="str">
+        <v>john@steelworks.com</v>
+      </c>
+      <c r="F2" t="str">
+        <v>+1-555-0201</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Stainless Steel, Mild Steel</v>
+      </c>
+      <c r="H2" t="str">
+        <v>Primary steel supplier</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>FAC002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Aluminum Solutions</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Detroit, MI</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Jane Doe</v>
+      </c>
+      <c r="E3" t="str">
+        <v>jane@alumsolutions.com</v>
+      </c>
+      <c r="F3" t="str">
+        <v>+1-555-0202</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Aluminum 6061, Aluminum 5052</v>
+      </c>
+      <c r="H3" t="str">
+        <v>High quality aluminum</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>FAC003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Copper Industries</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Phoenix, AZ</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Bob Johnson</v>
+      </c>
+      <c r="E4" t="str">
+        <v>bob@copperind.com</v>
+      </c>
+      <c r="F4" t="str">
+        <v>+1-555-0203</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Copper, Brass</v>
+      </c>
+      <c r="H4" t="str">
+        <v>Specialized copper products</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>factoryId</v>
+      </c>
+      <c r="D1" t="str">
+        <v>factoryName</v>
+      </c>
+      <c r="E1" t="str">
+        <v>material</v>
+      </c>
+      <c r="F1" t="str">
+        <v>size</v>
+      </c>
+      <c r="G1" t="str">
+        <v>thickness</v>
+      </c>
+      <c r="H1" t="str">
+        <v>qty</v>
+      </c>
+      <c r="I1" t="str">
+        <v>unitCost</v>
+      </c>
+      <c r="J1" t="str">
+        <v>totalCost</v>
+      </c>
+      <c r="K1" t="str">
+        <v>batchRef</v>
+      </c>
+      <c r="L1" t="str">
+        <v>notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>PUR001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2024-01-15</v>
+      </c>
+      <c r="C2" t="str">
+        <v>FAC001</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Steel Works Ltd</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Stainless Steel</v>
+      </c>
+      <c r="F2" t="str">
+        <v>2440x1220</v>
+      </c>
+      <c r="G2" t="str">
+        <v>3mm</v>
+      </c>
+      <c r="H2">
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>85.5</v>
+      </c>
+      <c r="J2">
+        <v>4275</v>
+      </c>
+      <c r="K2" t="str">
+        <v>BATCH-2024-001</v>
+      </c>
+      <c r="L2" t="str">
+        <v>Premium grade stainless steel</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>PUR002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2024-01-20</v>
+      </c>
+      <c r="C3" t="str">
+        <v>FAC002</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Aluminum Solutions</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Aluminum 6061</v>
+      </c>
+      <c r="F3" t="str">
+        <v>2440x1220</v>
+      </c>
+      <c r="G3" t="str">
+        <v>4mm</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="I3">
+        <v>95</v>
+      </c>
+      <c r="J3">
+        <v>2850</v>
+      </c>
+      <c r="K3" t="str">
+        <v>BATCH-2024-002</v>
+      </c>
+      <c r="L3" t="str">
+        <v>Aircraft grade aluminum</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>PUR003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2024-02-01</v>
+      </c>
+      <c r="C4" t="str">
+        <v>FAC001</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Steel Works Ltd</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Mild Steel</v>
+      </c>
+      <c r="F4" t="str">
+        <v>3000x1500</v>
+      </c>
+      <c r="G4" t="str">
+        <v>5mm</v>
+      </c>
+      <c r="H4">
+        <v>40</v>
+      </c>
+      <c r="I4">
+        <v>120</v>
+      </c>
+      <c r="J4">
+        <v>4800</v>
+      </c>
+      <c r="K4" t="str">
+        <v>BATCH-2024-003</v>
+      </c>
+      <c r="L4" t="str">
+        <v>Heavy duty mild steel</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add sample Categories and Products data to Excel file
Co-authored-by: ramarajan15 <11455808+ramarajan15@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/public/SheetCuttingBusinessTemplate.xlsx
+++ b/public/SheetCuttingBusinessTemplate.xlsx
@@ -7,6 +7,8 @@
     <sheet name="Customers" sheetId="2" r:id="rId2"/>
     <sheet name="Factories" sheetId="3" r:id="rId3"/>
     <sheet name="Purchases" sheetId="4" r:id="rId4"/>
+    <sheet name="Categories" sheetId="5" r:id="rId5"/>
+    <sheet name="Products" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -402,7 +404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -771,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -865,7 +867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -983,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -1143,4 +1145,364 @@
     <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>description</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>CAT001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Decorative Laminates</v>
+      </c>
+      <c r="C2" t="str">
+        <v>High-quality decorative laminates for furniture and interiors</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>CAT002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Industrial Laminates</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Durable laminates for industrial applications</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>CAT003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Compact Laminates</v>
+      </c>
+      <c r="C4" t="str">
+        <v>High-pressure compact laminates for heavy-duty use</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>CAT004</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Wood Finish Laminates</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Natural wood-finish laminate sheets</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>CAT005</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Solid Color Laminates</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Solid color laminate sheets for modern designs</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>categoryId</v>
+      </c>
+      <c r="D1" t="str">
+        <v>categoryName</v>
+      </c>
+      <c r="E1" t="str">
+        <v>length</v>
+      </c>
+      <c r="F1" t="str">
+        <v>width</v>
+      </c>
+      <c r="G1" t="str">
+        <v>thickness</v>
+      </c>
+      <c r="H1" t="str">
+        <v>area</v>
+      </c>
+      <c r="I1" t="str">
+        <v>unitCost</v>
+      </c>
+      <c r="J1" t="str">
+        <v>colour</v>
+      </c>
+      <c r="K1" t="str">
+        <v>weight</v>
+      </c>
+      <c r="L1" t="str">
+        <v>notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>PROD001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Premium Oak Laminate</v>
+      </c>
+      <c r="C2" t="str">
+        <v>CAT004</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Wood Finish Laminates</v>
+      </c>
+      <c r="E2">
+        <v>2440</v>
+      </c>
+      <c r="F2">
+        <v>1220</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2976800</v>
+      </c>
+      <c r="I2">
+        <v>0.0025</v>
+      </c>
+      <c r="J2" t="str">
+        <v>Oak Brown</v>
+      </c>
+      <c r="K2">
+        <v>15000</v>
+      </c>
+      <c r="L2" t="str">
+        <v>Popular wood finish, suitable for furniture</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>PROD002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Classic Walnut Laminate</v>
+      </c>
+      <c r="C3" t="str">
+        <v>CAT004</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Wood Finish Laminates</v>
+      </c>
+      <c r="E3">
+        <v>2440</v>
+      </c>
+      <c r="F3">
+        <v>1220</v>
+      </c>
+      <c r="G3">
+        <v>0.8</v>
+      </c>
+      <c r="H3">
+        <v>2976800</v>
+      </c>
+      <c r="I3">
+        <v>0.0028</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Dark Walnut</v>
+      </c>
+      <c r="K3">
+        <v>14000</v>
+      </c>
+      <c r="L3" t="str">
+        <v>Premium walnut finish</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>PROD003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Glossy White Laminate</v>
+      </c>
+      <c r="C4" t="str">
+        <v>CAT005</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Solid Color Laminates</v>
+      </c>
+      <c r="E4">
+        <v>2440</v>
+      </c>
+      <c r="F4">
+        <v>1220</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2976800</v>
+      </c>
+      <c r="I4">
+        <v>0.002</v>
+      </c>
+      <c r="J4" t="str">
+        <v>White</v>
+      </c>
+      <c r="K4">
+        <v>15000</v>
+      </c>
+      <c r="L4" t="str">
+        <v>High-gloss white finish</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>PROD004</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Matte Black Laminate</v>
+      </c>
+      <c r="C5" t="str">
+        <v>CAT005</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Solid Color Laminates</v>
+      </c>
+      <c r="E5">
+        <v>2440</v>
+      </c>
+      <c r="F5">
+        <v>1220</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>2976800</v>
+      </c>
+      <c r="I5">
+        <v>0.0022</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Black</v>
+      </c>
+      <c r="K5">
+        <v>15200</v>
+      </c>
+      <c r="L5" t="str">
+        <v>Matte black finish for modern designs</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>PROD005</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Industrial Grey Compact</v>
+      </c>
+      <c r="C6" t="str">
+        <v>CAT003</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Compact Laminates</v>
+      </c>
+      <c r="E6">
+        <v>3050</v>
+      </c>
+      <c r="F6">
+        <v>1300</v>
+      </c>
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>3965000</v>
+      </c>
+      <c r="I6">
+        <v>0.0045</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Grey</v>
+      </c>
+      <c r="K6">
+        <v>48000</v>
+      </c>
+      <c r="L6" t="str">
+        <v>High-pressure compact laminate for heavy-duty applications</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>PROD006</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Marble Effect Laminate</v>
+      </c>
+      <c r="C7" t="str">
+        <v>CAT001</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Decorative Laminates</v>
+      </c>
+      <c r="E7">
+        <v>2440</v>
+      </c>
+      <c r="F7">
+        <v>1220</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>2976800</v>
+      </c>
+      <c r="I7">
+        <v>0.0032</v>
+      </c>
+      <c r="J7" t="str">
+        <v>White Marble</v>
+      </c>
+      <c r="K7">
+        <v>15000</v>
+      </c>
+      <c r="L7" t="str">
+        <v>Realistic marble pattern for premium interiors</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>